<commit_message>
Changes done for deploy
</commit_message>
<xml_diff>
--- a/Camarilla_Calc.xlsx
+++ b/Camarilla_Calc.xlsx
@@ -3874,31 +3874,31 @@
         </is>
       </c>
       <c r="C3" s="27" t="n">
-        <v>4985.82</v>
+        <v>4857.4</v>
       </c>
       <c r="D3" s="28" t="n">
-        <v>201.66</v>
+        <v>197.44</v>
       </c>
       <c r="E3" s="27" t="n">
-        <v>44848.97</v>
+        <v>45269.56</v>
       </c>
       <c r="F3" s="27" t="n">
-        <v>67250.85000000001</v>
+        <v>68188.32000000001</v>
       </c>
       <c r="G3" s="43" t="n">
-        <v>716.86</v>
+        <v>689.97</v>
       </c>
       <c r="H3" s="28" t="n">
-        <v>224.41</v>
+        <v>220.84</v>
       </c>
       <c r="I3" s="28" t="n">
-        <v>164.06</v>
+        <v>161.98</v>
       </c>
       <c r="J3" s="28" t="n">
-        <v>1233.91</v>
+        <v>1184.44</v>
       </c>
       <c r="K3" s="28" t="n">
-        <v>177.67</v>
+        <v>173.11</v>
       </c>
       <c r="L3" s="41" t="inlineStr">
         <is>
@@ -3913,31 +3913,31 @@
         </is>
       </c>
       <c r="C4" s="27" t="n">
-        <v>4936.81</v>
+        <v>4843.7</v>
       </c>
       <c r="D4" s="28" t="n">
-        <v>200.03</v>
+        <v>195.87</v>
       </c>
       <c r="E4" s="27" t="n">
-        <v>44706.74</v>
+        <v>45151.13</v>
       </c>
       <c r="F4" s="27" t="n">
-        <v>66932.58</v>
+        <v>67880.81</v>
       </c>
       <c r="G4" s="43" t="n">
-        <v>712.3</v>
+        <v>688.2</v>
       </c>
       <c r="H4" s="28" t="n">
-        <v>223.53</v>
+        <v>219.78</v>
       </c>
       <c r="I4" s="28" t="n">
-        <v>163.66</v>
+        <v>161.43</v>
       </c>
       <c r="J4" s="28" t="n">
-        <v>1227.96</v>
+        <v>1179.92</v>
       </c>
       <c r="K4" s="28" t="n">
-        <v>176.86</v>
+        <v>172.74</v>
       </c>
       <c r="L4" s="41" t="inlineStr">
         <is>
@@ -3952,31 +3952,31 @@
         </is>
       </c>
       <c r="C5" s="29" t="n">
-        <v>4887.8</v>
+        <v>4830</v>
       </c>
       <c r="D5" s="30" t="n">
-        <v>198.4</v>
+        <v>194.3</v>
       </c>
       <c r="E5" s="29" t="n">
-        <v>44564.5</v>
+        <v>45032.7</v>
       </c>
       <c r="F5" s="29" t="n">
-        <v>66614.3</v>
+        <v>67573.3</v>
       </c>
       <c r="G5" s="45" t="n">
-        <v>707.73</v>
+        <v>686.4400000000001</v>
       </c>
       <c r="H5" s="30" t="n">
-        <v>222.64</v>
+        <v>218.73</v>
       </c>
       <c r="I5" s="30" t="n">
-        <v>163.26</v>
+        <v>160.89</v>
       </c>
       <c r="J5" s="30" t="n">
-        <v>1222.01</v>
+        <v>1175.4</v>
       </c>
       <c r="K5" s="30" t="n">
-        <v>176.05</v>
+        <v>172.38</v>
       </c>
       <c r="L5" s="46" t="inlineStr">
         <is>
@@ -3991,31 +3991,31 @@
         </is>
       </c>
       <c r="C6" s="25" t="n">
-        <v>4828.4</v>
+        <v>4813.5</v>
       </c>
       <c r="D6" s="26" t="n">
-        <v>196.45</v>
+        <v>192.4</v>
       </c>
       <c r="E6" s="25" t="n">
-        <v>44391.25</v>
+        <v>44891.35</v>
       </c>
       <c r="F6" s="25" t="n">
-        <v>66233.14999999999</v>
+        <v>67208.64999999999</v>
       </c>
       <c r="G6" s="47" t="n">
-        <v>702.47</v>
+        <v>684.3200000000001</v>
       </c>
       <c r="H6" s="26" t="n">
-        <v>221.6</v>
+        <v>217.46</v>
       </c>
       <c r="I6" s="26" t="n">
-        <v>162.78</v>
+        <v>160.25</v>
       </c>
       <c r="J6" s="26" t="n">
-        <v>1215.06</v>
+        <v>1169.9</v>
       </c>
       <c r="K6" s="26" t="n">
-        <v>175.08</v>
+        <v>171.94</v>
       </c>
       <c r="L6" s="48" t="inlineStr">
         <is>
@@ -4030,31 +4030,31 @@
         </is>
       </c>
       <c r="C7" s="27" t="n">
-        <v>4808.53</v>
+        <v>4807.98</v>
       </c>
       <c r="D7" s="28" t="n">
-        <v>195.8</v>
+        <v>191.76</v>
       </c>
       <c r="E7" s="27" t="n">
-        <v>44333.29</v>
+        <v>44844.06</v>
       </c>
       <c r="F7" s="27" t="n">
-        <v>66105.64</v>
+        <v>67086.66</v>
       </c>
       <c r="G7" s="43" t="n">
-        <v>700.7</v>
+        <v>683.61</v>
       </c>
       <c r="H7" s="28" t="n">
-        <v>221.25</v>
+        <v>217.04</v>
       </c>
       <c r="I7" s="28" t="n">
-        <v>162.62</v>
+        <v>160.03</v>
       </c>
       <c r="J7" s="28" t="n">
-        <v>1212.73</v>
+        <v>1168.06</v>
       </c>
       <c r="K7" s="28" t="n">
-        <v>174.75</v>
+        <v>171.79</v>
       </c>
       <c r="L7" s="41" t="inlineStr">
         <is>
@@ -4069,31 +4069,31 @@
         </is>
       </c>
       <c r="C8" s="27" t="n">
-        <v>4788.79</v>
+        <v>4802.5</v>
       </c>
       <c r="D8" s="28" t="n">
-        <v>195.15</v>
+        <v>191.13</v>
       </c>
       <c r="E8" s="27" t="n">
-        <v>44275.71</v>
+        <v>44797.08</v>
       </c>
       <c r="F8" s="27" t="n">
-        <v>65978.96000000001</v>
+        <v>66965.46000000001</v>
       </c>
       <c r="G8" s="43" t="n">
-        <v>698.95</v>
+        <v>682.91</v>
       </c>
       <c r="H8" s="28" t="n">
-        <v>220.9</v>
+        <v>216.62</v>
       </c>
       <c r="I8" s="28" t="n">
-        <v>162.46</v>
+        <v>159.82</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>1210.42</v>
+        <v>1166.23</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>174.43</v>
+        <v>171.65</v>
       </c>
       <c r="L8" s="41" t="inlineStr">
         <is>
@@ -4108,31 +4108,31 @@
         </is>
       </c>
       <c r="C9" s="27" t="n">
-        <v>4749.21</v>
+        <v>4791.5</v>
       </c>
       <c r="D9" s="28" t="n">
-        <v>193.85</v>
+        <v>189.87</v>
       </c>
       <c r="E9" s="27" t="n">
-        <v>44160.29</v>
+        <v>44702.92</v>
       </c>
       <c r="F9" s="27" t="n">
-        <v>65725.03999999999</v>
+        <v>66722.53999999999</v>
       </c>
       <c r="G9" s="43" t="n">
-        <v>695.45</v>
+        <v>681.49</v>
       </c>
       <c r="H9" s="28" t="n">
-        <v>220.2</v>
+        <v>215.78</v>
       </c>
       <c r="I9" s="28" t="n">
-        <v>162.14</v>
+        <v>159.38</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>1205.78</v>
+        <v>1162.57</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>173.77</v>
+        <v>171.35</v>
       </c>
       <c r="L9" s="41" t="inlineStr">
         <is>
@@ -4147,31 +4147,31 @@
         </is>
       </c>
       <c r="C10" s="27" t="n">
-        <v>4729.47</v>
+        <v>4786.02</v>
       </c>
       <c r="D10" s="28" t="n">
-        <v>193.2</v>
+        <v>189.24</v>
       </c>
       <c r="E10" s="27" t="n">
-        <v>44102.71</v>
+        <v>44655.94</v>
       </c>
       <c r="F10" s="27" t="n">
-        <v>65598.36</v>
+        <v>66601.34</v>
       </c>
       <c r="G10" s="43" t="n">
-        <v>693.7</v>
+        <v>680.79</v>
       </c>
       <c r="H10" s="28" t="n">
-        <v>219.85</v>
+        <v>215.36</v>
       </c>
       <c r="I10" s="28" t="n">
-        <v>161.98</v>
+        <v>159.17</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>1203.47</v>
+        <v>1160.74</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>173.45</v>
+        <v>171.21</v>
       </c>
       <c r="L10" s="41" t="inlineStr">
         <is>
@@ -4186,31 +4186,31 @@
         </is>
       </c>
       <c r="C11" s="29" t="n">
-        <v>4709.6</v>
+        <v>4780.5</v>
       </c>
       <c r="D11" s="30" t="n">
-        <v>192.55</v>
+        <v>188.6</v>
       </c>
       <c r="E11" s="29" t="n">
-        <v>44044.75</v>
+        <v>44608.65</v>
       </c>
       <c r="F11" s="29" t="n">
-        <v>65470.85</v>
+        <v>66479.35000000001</v>
       </c>
       <c r="G11" s="45" t="n">
-        <v>691.9299999999999</v>
+        <v>680.08</v>
       </c>
       <c r="H11" s="30" t="n">
-        <v>219.51</v>
+        <v>214.94</v>
       </c>
       <c r="I11" s="30" t="n">
-        <v>161.82</v>
+        <v>158.95</v>
       </c>
       <c r="J11" s="30" t="n">
-        <v>1201.14</v>
+        <v>1158.9</v>
       </c>
       <c r="K11" s="30" t="n">
-        <v>173.12</v>
+        <v>171.06</v>
       </c>
       <c r="L11" s="46" t="inlineStr">
         <is>
@@ -4225,31 +4225,31 @@
         </is>
       </c>
       <c r="C12" s="25" t="n">
-        <v>4650.2</v>
+        <v>4764</v>
       </c>
       <c r="D12" s="26" t="n">
-        <v>190.6</v>
+        <v>186.7</v>
       </c>
       <c r="E12" s="25" t="n">
-        <v>43871.5</v>
+        <v>44467.3</v>
       </c>
       <c r="F12" s="25" t="n">
-        <v>65089.7</v>
+        <v>66114.7</v>
       </c>
       <c r="G12" s="47" t="n">
-        <v>686.67</v>
+        <v>677.96</v>
       </c>
       <c r="H12" s="26" t="n">
-        <v>218.46</v>
+        <v>213.67</v>
       </c>
       <c r="I12" s="26" t="n">
-        <v>161.34</v>
+        <v>158.31</v>
       </c>
       <c r="J12" s="26" t="n">
-        <v>1194.18</v>
+        <v>1153.4</v>
       </c>
       <c r="K12" s="26" t="n">
-        <v>172.15</v>
+        <v>170.62</v>
       </c>
       <c r="L12" s="48" t="inlineStr">
         <is>
@@ -4264,31 +4264,31 @@
         </is>
       </c>
       <c r="C13" s="27" t="n">
-        <v>4601.19</v>
+        <v>4750.3</v>
       </c>
       <c r="D13" s="28" t="n">
-        <v>188.97</v>
+        <v>185.13</v>
       </c>
       <c r="E13" s="27" t="n">
-        <v>43729.26</v>
+        <v>44348.87</v>
       </c>
       <c r="F13" s="27" t="n">
-        <v>64771.42</v>
+        <v>65807.19</v>
       </c>
       <c r="G13" s="43" t="n">
-        <v>682.1</v>
+        <v>676.2</v>
       </c>
       <c r="H13" s="28" t="n">
-        <v>217.57</v>
+        <v>212.62</v>
       </c>
       <c r="I13" s="28" t="n">
-        <v>160.94</v>
+        <v>157.77</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>1188.24</v>
+        <v>1148.88</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>171.34</v>
+        <v>170.26</v>
       </c>
       <c r="L13" s="41" t="inlineStr">
         <is>
@@ -4303,31 +4303,31 @@
         </is>
       </c>
       <c r="C14" s="35" t="n">
-        <v>4552.18</v>
+        <v>4736.6</v>
       </c>
       <c r="D14" s="36" t="n">
-        <v>187.34</v>
+        <v>183.56</v>
       </c>
       <c r="E14" s="35" t="n">
-        <v>43587.03</v>
+        <v>44230.44</v>
       </c>
       <c r="F14" s="35" t="n">
-        <v>64453.15</v>
+        <v>65499.68</v>
       </c>
       <c r="G14" s="44" t="n">
-        <v>677.54</v>
+        <v>674.4299999999999</v>
       </c>
       <c r="H14" s="36" t="n">
-        <v>216.69</v>
+        <v>211.56</v>
       </c>
       <c r="I14" s="36" t="n">
-        <v>160.54</v>
+        <v>157.22</v>
       </c>
       <c r="J14" s="36" t="n">
-        <v>1182.29</v>
+        <v>1144.36</v>
       </c>
       <c r="K14" s="36" t="n">
-        <v>170.53</v>
+        <v>169.89</v>
       </c>
       <c r="L14" s="42" t="inlineStr">
         <is>
@@ -4417,19 +4417,19 @@
         </is>
       </c>
       <c r="C2" s="23" t="n">
-        <v>4920</v>
+        <v>4778</v>
       </c>
       <c r="D2" s="23" t="n">
-        <v>4967</v>
+        <v>4825</v>
       </c>
       <c r="E2" s="23" t="n">
-        <v>4751</v>
+        <v>4765</v>
       </c>
       <c r="F2" s="23" t="n">
-        <v>4769</v>
+        <v>4797</v>
       </c>
       <c r="G2" s="23" t="n">
-        <v>4844</v>
+        <v>4796</v>
       </c>
       <c r="H2" s="24" t="n"/>
     </row>
@@ -4445,19 +4445,19 @@
         </is>
       </c>
       <c r="C3" s="23" t="n">
-        <v>197.2</v>
+        <v>194.3</v>
       </c>
       <c r="D3" s="23" t="n">
-        <v>200</v>
+        <v>196.2</v>
       </c>
       <c r="E3" s="23" t="n">
-        <v>192.9</v>
+        <v>189.3</v>
       </c>
       <c r="F3" s="23" t="n">
-        <v>194.5</v>
+        <v>190.5</v>
       </c>
       <c r="G3" s="23" t="n">
-        <v>197.2</v>
+        <v>193.8</v>
       </c>
       <c r="H3" s="24" t="n"/>
     </row>
@@ -4473,19 +4473,19 @@
         </is>
       </c>
       <c r="C4" s="23" t="n">
-        <v>44756</v>
+        <v>44741</v>
       </c>
       <c r="D4" s="23" t="n">
-        <v>44780</v>
+        <v>44785</v>
       </c>
       <c r="E4" s="23" t="n">
-        <v>44150</v>
+        <v>44271</v>
       </c>
       <c r="F4" s="23" t="n">
-        <v>44218</v>
+        <v>44750</v>
       </c>
       <c r="G4" s="23" t="n">
-        <v>44683</v>
+        <v>44879</v>
       </c>
       <c r="H4" s="24" t="n"/>
     </row>
@@ -4501,19 +4501,19 @@
         </is>
       </c>
       <c r="C5" s="23" t="n">
-        <v>66455</v>
+        <v>67200</v>
       </c>
       <c r="D5" s="23" t="n">
-        <v>66633</v>
+        <v>67259</v>
       </c>
       <c r="E5" s="23" t="n">
-        <v>65247</v>
+        <v>65933</v>
       </c>
       <c r="F5" s="23" t="n">
-        <v>65852</v>
+        <v>66844</v>
       </c>
       <c r="G5" s="23" t="n">
-        <v>65603</v>
+        <v>67545</v>
       </c>
       <c r="H5" s="24" t="n"/>
     </row>
@@ -4529,19 +4529,19 @@
         </is>
       </c>
       <c r="C6" s="23" t="n">
-        <v>682.35</v>
+        <v>683.8</v>
       </c>
       <c r="D6" s="23" t="n">
-        <v>698.15</v>
+        <v>683.8</v>
       </c>
       <c r="E6" s="23" t="n">
-        <v>679</v>
+        <v>676.1</v>
       </c>
       <c r="F6" s="23" t="n">
-        <v>697.2</v>
+        <v>682.2</v>
       </c>
       <c r="G6" s="23" t="n">
-        <v>691.5</v>
+        <v>686.55</v>
       </c>
       <c r="H6" s="24" t="n"/>
     </row>
@@ -4557,19 +4557,19 @@
         </is>
       </c>
       <c r="C7" s="23" t="n">
-        <v>218.9</v>
+        <v>218.65</v>
       </c>
       <c r="D7" s="23" t="n">
-        <v>220.7</v>
+        <v>219.1</v>
       </c>
       <c r="E7" s="23" t="n">
-        <v>216.9</v>
+        <v>214.5</v>
       </c>
       <c r="F7" s="23" t="n">
-        <v>220.55</v>
+        <v>216.2</v>
       </c>
       <c r="G7" s="23" t="n">
-        <v>219.05</v>
+        <v>218.55</v>
       </c>
       <c r="H7" s="24" t="n"/>
     </row>
@@ -4585,19 +4585,19 @@
         </is>
       </c>
       <c r="C8" s="23" t="n">
-        <v>161.5</v>
+        <v>158.7</v>
       </c>
       <c r="D8" s="23" t="n">
-        <v>162.9</v>
+        <v>160.25</v>
       </c>
       <c r="E8" s="23" t="n">
-        <v>161.15</v>
+        <v>157.9</v>
       </c>
       <c r="F8" s="23" t="n">
-        <v>162.3</v>
+        <v>159.6</v>
       </c>
       <c r="G8" s="23" t="n">
-        <v>161.95</v>
+        <v>158.8</v>
       </c>
       <c r="H8" s="24" t="n"/>
     </row>
@@ -4613,19 +4613,19 @@
         </is>
       </c>
       <c r="C9" s="23" t="n">
-        <v>1192.4</v>
+        <v>1180.3</v>
       </c>
       <c r="D9" s="23" t="n">
-        <v>1209.3</v>
+        <v>1182</v>
       </c>
       <c r="E9" s="23" t="n">
-        <v>1184</v>
+        <v>1162</v>
       </c>
       <c r="F9" s="23" t="n">
-        <v>1208.1</v>
+        <v>1164.4</v>
       </c>
       <c r="G9" s="23" t="n">
-        <v>1199.3</v>
+        <v>1186.2</v>
       </c>
       <c r="H9" s="24" t="n"/>
     </row>
@@ -4641,19 +4641,19 @@
         </is>
       </c>
       <c r="C10" s="23" t="n">
-        <v>176.35</v>
+        <v>172.45</v>
       </c>
       <c r="D10" s="23" t="n">
-        <v>176.65</v>
+        <v>172.45</v>
       </c>
       <c r="E10" s="23" t="n">
-        <v>173.1</v>
+        <v>170.85</v>
       </c>
       <c r="F10" s="23" t="n">
-        <v>174.1</v>
+        <v>171.5</v>
       </c>
       <c r="G10" s="23" t="n">
-        <v>175.85</v>
+        <v>172.95</v>
       </c>
       <c r="H10" s="24" t="n"/>
     </row>

</xml_diff>

<commit_message>
Added changes for Scheduler
</commit_message>
<xml_diff>
--- a/Camarilla_Calc.xlsx
+++ b/Camarilla_Calc.xlsx
@@ -3886,16 +3886,16 @@
         <v>68188.32000000001</v>
       </c>
       <c r="G3" s="43" t="n">
-        <v>689.97</v>
+        <v>688.04</v>
       </c>
       <c r="H3" s="28" t="n">
-        <v>220.84</v>
+        <v>219.78</v>
       </c>
       <c r="I3" s="28" t="n">
-        <v>161.98</v>
+        <v>163.2</v>
       </c>
       <c r="J3" s="28" t="n">
-        <v>1184.44</v>
+        <v>1177.76</v>
       </c>
       <c r="K3" s="28" t="n">
         <v>173.11</v>
@@ -3925,19 +3925,19 @@
         <v>67880.81</v>
       </c>
       <c r="G4" s="43" t="n">
-        <v>688.2</v>
+        <v>686.09</v>
       </c>
       <c r="H4" s="28" t="n">
-        <v>219.78</v>
+        <v>218.72</v>
       </c>
       <c r="I4" s="28" t="n">
-        <v>161.43</v>
+        <v>162.52</v>
       </c>
       <c r="J4" s="28" t="n">
-        <v>1179.92</v>
+        <v>1172.78</v>
       </c>
       <c r="K4" s="28" t="n">
-        <v>172.74</v>
+        <v>172.58</v>
       </c>
       <c r="L4" s="41" t="inlineStr">
         <is>
@@ -3964,19 +3964,19 @@
         <v>67573.3</v>
       </c>
       <c r="G5" s="45" t="n">
-        <v>686.4400000000001</v>
+        <v>684.15</v>
       </c>
       <c r="H5" s="30" t="n">
-        <v>218.73</v>
+        <v>217.66</v>
       </c>
       <c r="I5" s="30" t="n">
-        <v>160.89</v>
+        <v>161.84</v>
       </c>
       <c r="J5" s="30" t="n">
-        <v>1175.4</v>
+        <v>1167.8</v>
       </c>
       <c r="K5" s="30" t="n">
-        <v>172.38</v>
+        <v>172.04</v>
       </c>
       <c r="L5" s="46" t="inlineStr">
         <is>
@@ -4003,19 +4003,19 @@
         <v>67208.64999999999</v>
       </c>
       <c r="G6" s="47" t="n">
-        <v>684.3200000000001</v>
+        <v>681.8200000000001</v>
       </c>
       <c r="H6" s="26" t="n">
-        <v>217.46</v>
+        <v>216.38</v>
       </c>
       <c r="I6" s="26" t="n">
-        <v>160.25</v>
+        <v>161.05</v>
       </c>
       <c r="J6" s="26" t="n">
-        <v>1169.9</v>
+        <v>1161.75</v>
       </c>
       <c r="K6" s="26" t="n">
-        <v>171.94</v>
+        <v>171.4</v>
       </c>
       <c r="L6" s="48" t="inlineStr">
         <is>
@@ -4042,19 +4042,19 @@
         <v>67086.66</v>
       </c>
       <c r="G7" s="43" t="n">
-        <v>683.61</v>
+        <v>681.05</v>
       </c>
       <c r="H7" s="28" t="n">
-        <v>217.04</v>
+        <v>215.95</v>
       </c>
       <c r="I7" s="28" t="n">
-        <v>160.03</v>
+        <v>160.78</v>
       </c>
       <c r="J7" s="28" t="n">
-        <v>1168.06</v>
+        <v>1159.73</v>
       </c>
       <c r="K7" s="28" t="n">
-        <v>171.79</v>
+        <v>171.18</v>
       </c>
       <c r="L7" s="41" t="inlineStr">
         <is>
@@ -4081,19 +4081,19 @@
         <v>66965.46000000001</v>
       </c>
       <c r="G8" s="43" t="n">
-        <v>682.91</v>
+        <v>680.27</v>
       </c>
       <c r="H8" s="28" t="n">
-        <v>216.62</v>
+        <v>215.53</v>
       </c>
       <c r="I8" s="28" t="n">
-        <v>159.82</v>
+        <v>160.52</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>1166.23</v>
+        <v>1157.72</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>171.65</v>
+        <v>170.97</v>
       </c>
       <c r="L8" s="41" t="inlineStr">
         <is>
@@ -4120,19 +4120,19 @@
         <v>66722.53999999999</v>
       </c>
       <c r="G9" s="43" t="n">
-        <v>681.49</v>
+        <v>678.73</v>
       </c>
       <c r="H9" s="28" t="n">
-        <v>215.78</v>
+        <v>214.67</v>
       </c>
       <c r="I9" s="28" t="n">
-        <v>159.38</v>
+        <v>159.98</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>1162.57</v>
+        <v>1153.68</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>171.35</v>
+        <v>170.53</v>
       </c>
       <c r="L9" s="41" t="inlineStr">
         <is>
@@ -4159,19 +4159,19 @@
         <v>66601.34</v>
       </c>
       <c r="G10" s="43" t="n">
-        <v>680.79</v>
+        <v>677.95</v>
       </c>
       <c r="H10" s="28" t="n">
-        <v>215.36</v>
+        <v>214.25</v>
       </c>
       <c r="I10" s="28" t="n">
-        <v>159.17</v>
+        <v>159.72</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>1160.74</v>
+        <v>1151.67</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>171.21</v>
+        <v>170.32</v>
       </c>
       <c r="L10" s="41" t="inlineStr">
         <is>
@@ -4198,19 +4198,19 @@
         <v>66479.35000000001</v>
       </c>
       <c r="G11" s="45" t="n">
-        <v>680.08</v>
+        <v>677.1799999999999</v>
       </c>
       <c r="H11" s="30" t="n">
-        <v>214.94</v>
+        <v>213.82</v>
       </c>
       <c r="I11" s="30" t="n">
-        <v>158.95</v>
+        <v>159.45</v>
       </c>
       <c r="J11" s="30" t="n">
-        <v>1158.9</v>
+        <v>1149.65</v>
       </c>
       <c r="K11" s="30" t="n">
-        <v>171.06</v>
+        <v>170.1</v>
       </c>
       <c r="L11" s="46" t="inlineStr">
         <is>
@@ -4237,19 +4237,19 @@
         <v>66114.7</v>
       </c>
       <c r="G12" s="47" t="n">
-        <v>677.96</v>
+        <v>674.85</v>
       </c>
       <c r="H12" s="26" t="n">
-        <v>213.67</v>
+        <v>212.54</v>
       </c>
       <c r="I12" s="26" t="n">
-        <v>158.31</v>
+        <v>158.66</v>
       </c>
       <c r="J12" s="26" t="n">
-        <v>1153.4</v>
+        <v>1143.6</v>
       </c>
       <c r="K12" s="26" t="n">
-        <v>170.62</v>
+        <v>169.46</v>
       </c>
       <c r="L12" s="48" t="inlineStr">
         <is>
@@ -4276,19 +4276,19 @@
         <v>65807.19</v>
       </c>
       <c r="G13" s="43" t="n">
-        <v>676.2</v>
+        <v>672.91</v>
       </c>
       <c r="H13" s="28" t="n">
-        <v>212.62</v>
+        <v>211.48</v>
       </c>
       <c r="I13" s="28" t="n">
-        <v>157.77</v>
+        <v>157.98</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>1148.88</v>
+        <v>1138.62</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>170.26</v>
+        <v>168.92</v>
       </c>
       <c r="L13" s="41" t="inlineStr">
         <is>
@@ -4315,19 +4315,19 @@
         <v>65499.68</v>
       </c>
       <c r="G14" s="44" t="n">
-        <v>674.4299999999999</v>
+        <v>670.96</v>
       </c>
       <c r="H14" s="36" t="n">
-        <v>211.56</v>
+        <v>210.42</v>
       </c>
       <c r="I14" s="36" t="n">
-        <v>157.22</v>
+        <v>157.3</v>
       </c>
       <c r="J14" s="36" t="n">
-        <v>1144.36</v>
+        <v>1133.64</v>
       </c>
       <c r="K14" s="36" t="n">
-        <v>169.89</v>
+        <v>168.39</v>
       </c>
       <c r="L14" s="42" t="inlineStr">
         <is>
@@ -4525,23 +4525,23 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>30APR2021</t>
+          <t>31MAR2021</t>
         </is>
       </c>
       <c r="C6" s="23" t="n">
-        <v>683.8</v>
+        <v>679.8</v>
       </c>
       <c r="D6" s="23" t="n">
-        <v>683.8</v>
+        <v>680.65</v>
       </c>
       <c r="E6" s="23" t="n">
-        <v>676.1</v>
+        <v>672.2</v>
       </c>
       <c r="F6" s="23" t="n">
-        <v>682.2</v>
+        <v>679.5</v>
       </c>
       <c r="G6" s="23" t="n">
-        <v>686.55</v>
+        <v>684.1</v>
       </c>
       <c r="H6" s="24" t="n"/>
     </row>
@@ -4553,23 +4553,23 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>30APR2021</t>
+          <t>31MAR2021</t>
         </is>
       </c>
       <c r="C7" s="23" t="n">
-        <v>218.65</v>
+        <v>218.35</v>
       </c>
       <c r="D7" s="23" t="n">
-        <v>219.1</v>
+        <v>218.35</v>
       </c>
       <c r="E7" s="23" t="n">
-        <v>214.5</v>
+        <v>213.7</v>
       </c>
       <c r="F7" s="23" t="n">
-        <v>216.2</v>
+        <v>215.1</v>
       </c>
       <c r="G7" s="23" t="n">
-        <v>218.55</v>
+        <v>217.8</v>
       </c>
       <c r="H7" s="24" t="n"/>
     </row>
@@ -4581,23 +4581,23 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>30APR2021</t>
+          <t>31MAR2021</t>
         </is>
       </c>
       <c r="C8" s="23" t="n">
+        <v>158.6</v>
+      </c>
+      <c r="D8" s="23" t="n">
+        <v>160.5</v>
+      </c>
+      <c r="E8" s="23" t="n">
+        <v>157.6</v>
+      </c>
+      <c r="F8" s="23" t="n">
+        <v>160.25</v>
+      </c>
+      <c r="G8" s="23" t="n">
         <v>158.7</v>
-      </c>
-      <c r="D8" s="23" t="n">
-        <v>160.25</v>
-      </c>
-      <c r="E8" s="23" t="n">
-        <v>157.9</v>
-      </c>
-      <c r="F8" s="23" t="n">
-        <v>159.6</v>
-      </c>
-      <c r="G8" s="23" t="n">
-        <v>158.8</v>
       </c>
       <c r="H8" s="24" t="n"/>
     </row>
@@ -4609,23 +4609,23 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>30APR2021</t>
+          <t>31MAR2021</t>
         </is>
       </c>
       <c r="C9" s="23" t="n">
-        <v>1180.3</v>
+        <v>1174</v>
       </c>
       <c r="D9" s="23" t="n">
-        <v>1182</v>
+        <v>1174.8</v>
       </c>
       <c r="E9" s="23" t="n">
-        <v>1162</v>
+        <v>1152.8</v>
       </c>
       <c r="F9" s="23" t="n">
-        <v>1164.4</v>
+        <v>1155.7</v>
       </c>
       <c r="G9" s="23" t="n">
-        <v>1186.2</v>
+        <v>1181.3</v>
       </c>
       <c r="H9" s="24" t="n"/>
     </row>
@@ -4637,23 +4637,23 @@
       </c>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>30APR2021</t>
+          <t>31MAR2021</t>
         </is>
       </c>
       <c r="C10" s="23" t="n">
-        <v>172.45</v>
+        <v>172.4</v>
       </c>
       <c r="D10" s="23" t="n">
-        <v>172.45</v>
+        <v>172.4</v>
       </c>
       <c r="E10" s="23" t="n">
-        <v>170.85</v>
+        <v>170.05</v>
       </c>
       <c r="F10" s="23" t="n">
-        <v>171.5</v>
+        <v>170.75</v>
       </c>
       <c r="G10" s="23" t="n">
-        <v>172.95</v>
+        <v>172.9</v>
       </c>
       <c r="H10" s="24" t="n"/>
     </row>

</xml_diff>

<commit_message>
Changes for FLASK implementation
</commit_message>
<xml_diff>
--- a/Camarilla_Calc.xlsx
+++ b/Camarilla_Calc.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8385" tabRatio="600" firstSheet="4" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Oct06" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Oct07" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Oct10" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Oct11" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Oct06" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Oct07" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Oct10" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Oct11" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511" fullCalcOnLoad="1"/>
@@ -3874,31 +3874,31 @@
         </is>
       </c>
       <c r="C3" s="27" t="n">
-        <v>4857.4</v>
+        <v>4639.71</v>
       </c>
       <c r="D3" s="28" t="n">
-        <v>197.44</v>
+        <v>197.36</v>
       </c>
       <c r="E3" s="27" t="n">
-        <v>45269.56</v>
+        <v>46796.15</v>
       </c>
       <c r="F3" s="27" t="n">
-        <v>68188.32000000001</v>
+        <v>67463.37</v>
       </c>
       <c r="G3" s="43" t="n">
-        <v>688.04</v>
+        <v>693.75</v>
       </c>
       <c r="H3" s="28" t="n">
-        <v>219.78</v>
+        <v>226.76</v>
       </c>
       <c r="I3" s="28" t="n">
-        <v>163.2</v>
+        <v>165.46</v>
       </c>
       <c r="J3" s="28" t="n">
-        <v>1177.76</v>
+        <v>1247.72</v>
       </c>
       <c r="K3" s="28" t="n">
-        <v>173.11</v>
+        <v>185.74</v>
       </c>
       <c r="L3" s="41" t="inlineStr">
         <is>
@@ -3913,31 +3913,31 @@
         </is>
       </c>
       <c r="C4" s="27" t="n">
-        <v>4843.7</v>
+        <v>4602.58</v>
       </c>
       <c r="D4" s="28" t="n">
-        <v>195.87</v>
+        <v>196.14</v>
       </c>
       <c r="E4" s="27" t="n">
-        <v>45151.13</v>
+        <v>46711.25</v>
       </c>
       <c r="F4" s="27" t="n">
-        <v>67880.81</v>
+        <v>67161.99000000001</v>
       </c>
       <c r="G4" s="43" t="n">
-        <v>686.09</v>
+        <v>692.17</v>
       </c>
       <c r="H4" s="28" t="n">
-        <v>218.72</v>
+        <v>225.5</v>
       </c>
       <c r="I4" s="28" t="n">
-        <v>162.52</v>
+        <v>165.12</v>
       </c>
       <c r="J4" s="28" t="n">
-        <v>1172.78</v>
+        <v>1240.62</v>
       </c>
       <c r="K4" s="28" t="n">
-        <v>172.58</v>
+        <v>185.12</v>
       </c>
       <c r="L4" s="41" t="inlineStr">
         <is>
@@ -3952,31 +3952,31 @@
         </is>
       </c>
       <c r="C5" s="29" t="n">
-        <v>4830</v>
+        <v>4565.45</v>
       </c>
       <c r="D5" s="30" t="n">
-        <v>194.3</v>
+        <v>194.92</v>
       </c>
       <c r="E5" s="29" t="n">
-        <v>45032.7</v>
+        <v>46626.35</v>
       </c>
       <c r="F5" s="29" t="n">
-        <v>67573.3</v>
+        <v>66860.60000000001</v>
       </c>
       <c r="G5" s="45" t="n">
-        <v>684.15</v>
+        <v>690.59</v>
       </c>
       <c r="H5" s="30" t="n">
-        <v>217.66</v>
+        <v>224.23</v>
       </c>
       <c r="I5" s="30" t="n">
-        <v>161.84</v>
+        <v>164.77</v>
       </c>
       <c r="J5" s="30" t="n">
-        <v>1167.8</v>
+        <v>1233.51</v>
       </c>
       <c r="K5" s="30" t="n">
-        <v>172.04</v>
+        <v>184.51</v>
       </c>
       <c r="L5" s="46" t="inlineStr">
         <is>
@@ -3991,31 +3991,31 @@
         </is>
       </c>
       <c r="C6" s="25" t="n">
-        <v>4813.5</v>
+        <v>4521.73</v>
       </c>
       <c r="D6" s="26" t="n">
-        <v>192.4</v>
+        <v>193.46</v>
       </c>
       <c r="E6" s="25" t="n">
-        <v>44891.35</v>
+        <v>46522.68</v>
       </c>
       <c r="F6" s="25" t="n">
-        <v>67208.64999999999</v>
+        <v>66494.3</v>
       </c>
       <c r="G6" s="47" t="n">
-        <v>681.8200000000001</v>
+        <v>688.7</v>
       </c>
       <c r="H6" s="26" t="n">
-        <v>216.38</v>
+        <v>222.69</v>
       </c>
       <c r="I6" s="26" t="n">
-        <v>161.05</v>
+        <v>164.36</v>
       </c>
       <c r="J6" s="26" t="n">
-        <v>1161.75</v>
+        <v>1224.91</v>
       </c>
       <c r="K6" s="26" t="n">
-        <v>171.4</v>
+        <v>183.78</v>
       </c>
       <c r="L6" s="48" t="inlineStr">
         <is>
@@ -4030,31 +4030,31 @@
         </is>
       </c>
       <c r="C7" s="27" t="n">
-        <v>4807.98</v>
+        <v>4507.1</v>
       </c>
       <c r="D7" s="28" t="n">
-        <v>191.76</v>
+        <v>192.97</v>
       </c>
       <c r="E7" s="27" t="n">
-        <v>44844.06</v>
+        <v>46487.99</v>
       </c>
       <c r="F7" s="27" t="n">
-        <v>67086.66</v>
+        <v>66371.75999999999</v>
       </c>
       <c r="G7" s="43" t="n">
-        <v>681.05</v>
+        <v>688.0599999999999</v>
       </c>
       <c r="H7" s="28" t="n">
-        <v>215.95</v>
+        <v>222.17</v>
       </c>
       <c r="I7" s="28" t="n">
-        <v>160.78</v>
+        <v>164.22</v>
       </c>
       <c r="J7" s="28" t="n">
-        <v>1159.73</v>
+        <v>1222.03</v>
       </c>
       <c r="K7" s="28" t="n">
-        <v>171.18</v>
+        <v>183.53</v>
       </c>
       <c r="L7" s="41" t="inlineStr">
         <is>
@@ -4069,31 +4069,31 @@
         </is>
       </c>
       <c r="C8" s="27" t="n">
-        <v>4802.5</v>
+        <v>4492.56</v>
       </c>
       <c r="D8" s="28" t="n">
-        <v>191.13</v>
+        <v>192.49</v>
       </c>
       <c r="E8" s="27" t="n">
-        <v>44797.08</v>
+        <v>46453.53</v>
       </c>
       <c r="F8" s="27" t="n">
-        <v>66965.46000000001</v>
+        <v>66250.00999999999</v>
       </c>
       <c r="G8" s="43" t="n">
-        <v>680.27</v>
+        <v>687.4299999999999</v>
       </c>
       <c r="H8" s="28" t="n">
-        <v>215.53</v>
+        <v>221.66</v>
       </c>
       <c r="I8" s="28" t="n">
-        <v>160.52</v>
+        <v>164.09</v>
       </c>
       <c r="J8" s="28" t="n">
-        <v>1157.72</v>
+        <v>1219.17</v>
       </c>
       <c r="K8" s="28" t="n">
-        <v>170.97</v>
+        <v>183.29</v>
       </c>
       <c r="L8" s="41" t="inlineStr">
         <is>
@@ -4108,31 +4108,31 @@
         </is>
       </c>
       <c r="C9" s="27" t="n">
-        <v>4791.5</v>
+        <v>4463.44</v>
       </c>
       <c r="D9" s="28" t="n">
-        <v>189.87</v>
+        <v>191.51</v>
       </c>
       <c r="E9" s="27" t="n">
-        <v>44702.92</v>
+        <v>46384.47</v>
       </c>
       <c r="F9" s="27" t="n">
-        <v>66722.53999999999</v>
+        <v>66005.99000000001</v>
       </c>
       <c r="G9" s="43" t="n">
-        <v>678.73</v>
+        <v>686.17</v>
       </c>
       <c r="H9" s="28" t="n">
-        <v>214.67</v>
+        <v>220.64</v>
       </c>
       <c r="I9" s="28" t="n">
-        <v>159.98</v>
+        <v>163.81</v>
       </c>
       <c r="J9" s="28" t="n">
-        <v>1153.68</v>
+        <v>1213.43</v>
       </c>
       <c r="K9" s="28" t="n">
-        <v>170.53</v>
+        <v>182.81</v>
       </c>
       <c r="L9" s="41" t="inlineStr">
         <is>
@@ -4147,31 +4147,31 @@
         </is>
       </c>
       <c r="C10" s="27" t="n">
-        <v>4786.02</v>
+        <v>4448.9</v>
       </c>
       <c r="D10" s="28" t="n">
-        <v>189.24</v>
+        <v>191.03</v>
       </c>
       <c r="E10" s="27" t="n">
-        <v>44655.94</v>
+        <v>46350.01</v>
       </c>
       <c r="F10" s="27" t="n">
-        <v>66601.34</v>
+        <v>65884.24000000001</v>
       </c>
       <c r="G10" s="43" t="n">
-        <v>677.95</v>
+        <v>685.54</v>
       </c>
       <c r="H10" s="28" t="n">
-        <v>214.25</v>
+        <v>220.13</v>
       </c>
       <c r="I10" s="28" t="n">
-        <v>159.72</v>
+        <v>163.68</v>
       </c>
       <c r="J10" s="28" t="n">
-        <v>1151.67</v>
+        <v>1210.57</v>
       </c>
       <c r="K10" s="28" t="n">
-        <v>170.32</v>
+        <v>182.57</v>
       </c>
       <c r="L10" s="41" t="inlineStr">
         <is>
@@ -4186,31 +4186,31 @@
         </is>
       </c>
       <c r="C11" s="29" t="n">
-        <v>4780.5</v>
+        <v>4434.27</v>
       </c>
       <c r="D11" s="30" t="n">
-        <v>188.6</v>
+        <v>190.54</v>
       </c>
       <c r="E11" s="29" t="n">
-        <v>44608.65</v>
+        <v>46315.32</v>
       </c>
       <c r="F11" s="29" t="n">
-        <v>66479.35000000001</v>
+        <v>65761.7</v>
       </c>
       <c r="G11" s="45" t="n">
-        <v>677.1799999999999</v>
+        <v>684.9</v>
       </c>
       <c r="H11" s="30" t="n">
-        <v>213.82</v>
+        <v>219.61</v>
       </c>
       <c r="I11" s="30" t="n">
-        <v>159.45</v>
+        <v>163.54</v>
       </c>
       <c r="J11" s="30" t="n">
-        <v>1149.65</v>
+        <v>1207.69</v>
       </c>
       <c r="K11" s="30" t="n">
-        <v>170.1</v>
+        <v>182.32</v>
       </c>
       <c r="L11" s="46" t="inlineStr">
         <is>
@@ -4225,31 +4225,31 @@
         </is>
       </c>
       <c r="C12" s="25" t="n">
-        <v>4764</v>
+        <v>4390.55</v>
       </c>
       <c r="D12" s="26" t="n">
-        <v>186.7</v>
+        <v>189.08</v>
       </c>
       <c r="E12" s="25" t="n">
-        <v>44467.3</v>
+        <v>46211.65</v>
       </c>
       <c r="F12" s="25" t="n">
-        <v>66114.7</v>
+        <v>65395.4</v>
       </c>
       <c r="G12" s="47" t="n">
-        <v>674.85</v>
+        <v>683</v>
       </c>
       <c r="H12" s="26" t="n">
-        <v>212.54</v>
+        <v>218.07</v>
       </c>
       <c r="I12" s="26" t="n">
-        <v>158.66</v>
+        <v>163.12</v>
       </c>
       <c r="J12" s="26" t="n">
-        <v>1143.6</v>
+        <v>1199.08</v>
       </c>
       <c r="K12" s="26" t="n">
-        <v>169.46</v>
+        <v>181.59</v>
       </c>
       <c r="L12" s="48" t="inlineStr">
         <is>
@@ -4264,31 +4264,31 @@
         </is>
       </c>
       <c r="C13" s="27" t="n">
-        <v>4750.3</v>
+        <v>4353.42</v>
       </c>
       <c r="D13" s="28" t="n">
-        <v>185.13</v>
+        <v>187.86</v>
       </c>
       <c r="E13" s="27" t="n">
-        <v>44348.87</v>
+        <v>46126.75</v>
       </c>
       <c r="F13" s="27" t="n">
-        <v>65807.19</v>
+        <v>65094.01</v>
       </c>
       <c r="G13" s="43" t="n">
-        <v>672.91</v>
+        <v>681.4299999999999</v>
       </c>
       <c r="H13" s="28" t="n">
-        <v>211.48</v>
+        <v>216.8</v>
       </c>
       <c r="I13" s="28" t="n">
-        <v>157.98</v>
+        <v>162.78</v>
       </c>
       <c r="J13" s="28" t="n">
-        <v>1138.62</v>
+        <v>1191.98</v>
       </c>
       <c r="K13" s="28" t="n">
-        <v>168.92</v>
+        <v>180.98</v>
       </c>
       <c r="L13" s="41" t="inlineStr">
         <is>
@@ -4303,31 +4303,31 @@
         </is>
       </c>
       <c r="C14" s="35" t="n">
-        <v>4736.6</v>
+        <v>4316.29</v>
       </c>
       <c r="D14" s="36" t="n">
-        <v>183.56</v>
+        <v>186.64</v>
       </c>
       <c r="E14" s="35" t="n">
-        <v>44230.44</v>
+        <v>46041.85</v>
       </c>
       <c r="F14" s="35" t="n">
-        <v>65499.68</v>
+        <v>64792.63</v>
       </c>
       <c r="G14" s="44" t="n">
-        <v>670.96</v>
+        <v>679.85</v>
       </c>
       <c r="H14" s="36" t="n">
-        <v>210.42</v>
+        <v>215.54</v>
       </c>
       <c r="I14" s="36" t="n">
-        <v>157.3</v>
+        <v>162.44</v>
       </c>
       <c r="J14" s="36" t="n">
-        <v>1133.64</v>
+        <v>1184.88</v>
       </c>
       <c r="K14" s="36" t="n">
-        <v>168.39</v>
+        <v>180.36</v>
       </c>
       <c r="L14" s="42" t="inlineStr">
         <is>
@@ -4413,23 +4413,23 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>19MAR2021</t>
+          <t>19APR2021</t>
         </is>
       </c>
       <c r="C2" s="23" t="n">
-        <v>4778</v>
+        <v>4442</v>
       </c>
       <c r="D2" s="23" t="n">
-        <v>4825</v>
+        <v>4562</v>
       </c>
       <c r="E2" s="23" t="n">
-        <v>4765</v>
+        <v>4403</v>
       </c>
       <c r="F2" s="23" t="n">
-        <v>4797</v>
+        <v>4478</v>
       </c>
       <c r="G2" s="23" t="n">
-        <v>4796</v>
+        <v>4434</v>
       </c>
       <c r="H2" s="24" t="n"/>
     </row>
@@ -4441,23 +4441,23 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>26MAR2021</t>
+          <t>27APR2021</t>
         </is>
       </c>
       <c r="C3" s="23" t="n">
-        <v>194.3</v>
+        <v>190</v>
       </c>
       <c r="D3" s="23" t="n">
-        <v>196.2</v>
+        <v>195.3</v>
       </c>
       <c r="E3" s="23" t="n">
-        <v>189.3</v>
+        <v>190</v>
       </c>
       <c r="F3" s="23" t="n">
-        <v>190.5</v>
+        <v>192</v>
       </c>
       <c r="G3" s="23" t="n">
-        <v>193.8</v>
+        <v>189.1</v>
       </c>
       <c r="H3" s="24" t="n"/>
     </row>
@@ -4469,23 +4469,23 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>05APR2021</t>
+          <t>04JUN2021</t>
         </is>
       </c>
       <c r="C4" s="23" t="n">
-        <v>44741</v>
+        <v>46545</v>
       </c>
       <c r="D4" s="23" t="n">
-        <v>44785</v>
+        <v>46777</v>
       </c>
       <c r="E4" s="23" t="n">
-        <v>44271</v>
+        <v>46400</v>
       </c>
       <c r="F4" s="23" t="n">
-        <v>44750</v>
+        <v>46419</v>
       </c>
       <c r="G4" s="23" t="n">
-        <v>44879</v>
+        <v>46593</v>
       </c>
       <c r="H4" s="24" t="n"/>
     </row>
@@ -4501,19 +4501,19 @@
         </is>
       </c>
       <c r="C5" s="23" t="n">
-        <v>67200</v>
+        <v>66786</v>
       </c>
       <c r="D5" s="23" t="n">
-        <v>67259</v>
+        <v>67293</v>
       </c>
       <c r="E5" s="23" t="n">
-        <v>65933</v>
+        <v>65961</v>
       </c>
       <c r="F5" s="23" t="n">
-        <v>66844</v>
+        <v>66128</v>
       </c>
       <c r="G5" s="23" t="n">
-        <v>67545</v>
+        <v>66983</v>
       </c>
       <c r="H5" s="24" t="n"/>
     </row>
@@ -4525,23 +4525,23 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>31MAR2021</t>
+          <t>30APR2021</t>
         </is>
       </c>
       <c r="C6" s="23" t="n">
-        <v>679.8</v>
+        <v>686</v>
       </c>
       <c r="D6" s="23" t="n">
-        <v>680.65</v>
+        <v>688.65</v>
       </c>
       <c r="E6" s="23" t="n">
-        <v>672.2</v>
+        <v>681.75</v>
       </c>
       <c r="F6" s="23" t="n">
-        <v>679.5</v>
+        <v>686.8</v>
       </c>
       <c r="G6" s="23" t="n">
-        <v>684.1</v>
+        <v>689.85</v>
       </c>
       <c r="H6" s="24" t="n"/>
     </row>
@@ -4553,23 +4553,23 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>31MAR2021</t>
+          <t>30APR2021</t>
         </is>
       </c>
       <c r="C7" s="23" t="n">
-        <v>218.35</v>
+        <v>226.3</v>
       </c>
       <c r="D7" s="23" t="n">
-        <v>218.35</v>
+        <v>226.3</v>
       </c>
       <c r="E7" s="23" t="n">
-        <v>213.7</v>
+        <v>220.7</v>
       </c>
       <c r="F7" s="23" t="n">
-        <v>215.1</v>
+        <v>221.15</v>
       </c>
       <c r="G7" s="23" t="n">
-        <v>217.8</v>
+        <v>227.7</v>
       </c>
       <c r="H7" s="24" t="n"/>
     </row>
@@ -4581,23 +4581,23 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>31MAR2021</t>
+          <t>30APR2021</t>
         </is>
       </c>
       <c r="C8" s="23" t="n">
-        <v>158.6</v>
+        <v>164</v>
       </c>
       <c r="D8" s="23" t="n">
-        <v>160.5</v>
+        <v>164.4</v>
       </c>
       <c r="E8" s="23" t="n">
-        <v>157.6</v>
+        <v>162.9</v>
       </c>
       <c r="F8" s="23" t="n">
-        <v>160.25</v>
+        <v>163.95</v>
       </c>
       <c r="G8" s="23" t="n">
-        <v>158.7</v>
+        <v>164.45</v>
       </c>
       <c r="H8" s="24" t="n"/>
     </row>
@@ -4609,23 +4609,23 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>31MAR2021</t>
+          <t>30APR2021</t>
         </is>
       </c>
       <c r="C9" s="23" t="n">
-        <v>1174</v>
+        <v>1243</v>
       </c>
       <c r="D9" s="23" t="n">
-        <v>1174.8</v>
+        <v>1243</v>
       </c>
       <c r="E9" s="23" t="n">
-        <v>1152.8</v>
+        <v>1211.7</v>
       </c>
       <c r="F9" s="23" t="n">
-        <v>1155.7</v>
+        <v>1216.3</v>
       </c>
       <c r="G9" s="23" t="n">
-        <v>1181.3</v>
+        <v>1252.7</v>
       </c>
       <c r="H9" s="24" t="n"/>
     </row>
@@ -4637,23 +4637,23 @@
       </c>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>31MAR2021</t>
+          <t>30APR2021</t>
         </is>
       </c>
       <c r="C10" s="23" t="n">
-        <v>172.4</v>
+        <v>181.5</v>
       </c>
       <c r="D10" s="23" t="n">
-        <v>172.4</v>
+        <v>183.3</v>
       </c>
       <c r="E10" s="23" t="n">
-        <v>170.05</v>
+        <v>180.65</v>
       </c>
       <c r="F10" s="23" t="n">
-        <v>170.75</v>
+        <v>183.05</v>
       </c>
       <c r="G10" s="23" t="n">
-        <v>172.9</v>
+        <v>182.25</v>
       </c>
       <c r="H10" s="24" t="n"/>
     </row>

</xml_diff>